<commit_message>
New sheet for testing
</commit_message>
<xml_diff>
--- a/tests/test_files/1_lab_journal_new.xlsx
+++ b/tests/test_files/1_lab_journal_new.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet2!$A$1:$M$25</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="104">
   <si>
     <t xml:space="preserve">day</t>
   </si>
@@ -296,6 +297,9 @@
   </si>
   <si>
     <t xml:space="preserve">.jpeg file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.09.2023</t>
   </si>
   <si>
     <t xml:space="preserve">data0740</t>
@@ -588,10 +592,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -840,20 +844,23 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" s="15" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="C13" s="15"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="1"/>
+      <c r="H13" s="15"/>
       <c r="I13" s="13" t="s">
         <v>47</v>
       </c>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -1058,80 +1065,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I27" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I30" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:M2"/>
@@ -1147,4 +1084,261 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="1" width="15.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="1" width="30.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="15.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Method for detecting missing files
</commit_message>
<xml_diff>
--- a/tests/test_files/1_lab_journal_new.xlsx
+++ b/tests/test_files/1_lab_journal_new.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="106">
   <si>
     <t xml:space="preserve">day</t>
   </si>
@@ -194,7 +194,7 @@
     <t xml:space="preserve">stm_sxm</t>
   </si>
   <si>
-    <t xml:space="preserve">Stm-nanonis-sxm</t>
+    <t xml:space="preserve">stm-nanonis-sxm</t>
   </si>
   <si>
     <t xml:space="preserve">STM Nanonis .sxm file</t>
@@ -236,7 +236,7 @@
     <t xml:space="preserve">cv_ec4</t>
   </si>
   <si>
-    <t xml:space="preserve">CV_153505_1</t>
+    <t xml:space="preserve">CV_153505_ 1</t>
   </si>
   <si>
     <t xml:space="preserve">O2</t>
@@ -251,7 +251,7 @@
     <t xml:space="preserve">Cyclic Voltammetry Nordic Electrochemistry EC-4 Cycle 1</t>
   </si>
   <si>
-    <t xml:space="preserve">CV_153605_2</t>
+    <t xml:space="preserve">CV_153605_ 2</t>
   </si>
   <si>
     <t xml:space="preserve">gas ambient</t>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t xml:space="preserve">FFT ECSTM (LabVIEW) - try to show only up to 2 kHz to visualize most relevant noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_missing_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_missing_2</t>
   </si>
 </sst>
 </file>
@@ -594,8 +600,8 @@
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1094,7 +1100,7 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1304,6 +1310,17 @@
       </c>
       <c r="I10" s="13" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>